<commit_message>
Make changes to d_error calculation in PID.cpp, based on suggestion from reviewer. Change cooeficient data tuned from 1st time, in main.cpp. Add the tuning log data from first try, which perform better in simulation. Update README.
</commit_message>
<xml_diff>
--- a/PID_log.xlsx
+++ b/PID_log.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10845"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10845" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="789779" sheetId="4" r:id="rId1"/>
+    <sheet name="2ND TUNING" sheetId="4" r:id="rId1"/>
+    <sheet name="1ST TUNING" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Kp</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>best_err_0</t>
+  </si>
+  <si>
+    <t>best_err</t>
   </si>
 </sst>
 </file>
@@ -104,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -112,6 +116,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,9 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I706"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K509" sqref="K509"/>
+      <selection pane="bottomLeft" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20917,4 +20922,3677 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G159"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.24</v>
+      </c>
+      <c r="B2">
+        <v>2E-3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.04</v>
+      </c>
+      <c r="E2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F2">
+        <v>0.44</v>
+      </c>
+      <c r="G2">
+        <v>492.30799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.24</v>
+      </c>
+      <c r="B3">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F3">
+        <v>0.44</v>
+      </c>
+      <c r="G3">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.24</v>
+      </c>
+      <c r="B4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E4">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F4">
+        <v>0.44</v>
+      </c>
+      <c r="G4">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.24</v>
+      </c>
+      <c r="B5">
+        <v>2E-3</v>
+      </c>
+      <c r="C5">
+        <v>2.44</v>
+      </c>
+      <c r="D5">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F5">
+        <v>0.44</v>
+      </c>
+      <c r="G5">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.24</v>
+      </c>
+      <c r="B6">
+        <v>2E-3</v>
+      </c>
+      <c r="C6">
+        <v>1.56</v>
+      </c>
+      <c r="D6">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E6">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F6">
+        <v>0.44</v>
+      </c>
+      <c r="G6">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="B7">
+        <v>2E-3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E7">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F7">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G7">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="B8">
+        <v>2E-3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E8">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F8">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G8">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.24</v>
+      </c>
+      <c r="B9">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="E9">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F9">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G9">
+        <v>457.32499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.24</v>
+      </c>
+      <c r="B10">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <v>2.3959999999999999</v>
+      </c>
+      <c r="D10">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="E10">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F10">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G10">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.24</v>
+      </c>
+      <c r="B11">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="D11">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="E11">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F11">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G11">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.27960000000000002</v>
+      </c>
+      <c r="B12">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="E12">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F12">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G12">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="B13">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F13">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G13">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.24</v>
+      </c>
+      <c r="B14">
+        <v>2.7560000000000002E-3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E14">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F14">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G14">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.24</v>
+      </c>
+      <c r="B15">
+        <v>1.964E-3</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E15">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="F15">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G15">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.24</v>
+      </c>
+      <c r="B16">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C16">
+        <v>2.3563999999999998</v>
+      </c>
+      <c r="D16">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E16">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F16">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G16">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.24</v>
+      </c>
+      <c r="B17">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C17">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D17">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E17">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F17">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="G17">
+        <v>452.25900000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.27564</v>
+      </c>
+      <c r="B18">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D18">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E18">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F18">
+        <v>0.39204</v>
+      </c>
+      <c r="G18">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.20436000000000001</v>
+      </c>
+      <c r="B19">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C19">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D19">
+        <v>3.5639999999999998E-2</v>
+      </c>
+      <c r="E19">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F19">
+        <v>0.39204</v>
+      </c>
+      <c r="G19">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.24</v>
+      </c>
+      <c r="B20">
+        <v>2.7163999999999999E-3</v>
+      </c>
+      <c r="C20">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D20">
+        <v>3.2076E-2</v>
+      </c>
+      <c r="E20">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F20">
+        <v>0.39204</v>
+      </c>
+      <c r="G20">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.24</v>
+      </c>
+      <c r="B21">
+        <v>2.0035999999999999E-3</v>
+      </c>
+      <c r="C21">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D21">
+        <v>3.2076E-2</v>
+      </c>
+      <c r="E21">
+        <v>3.5639999999999999E-4</v>
+      </c>
+      <c r="F21">
+        <v>0.39204</v>
+      </c>
+      <c r="G21">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.24</v>
+      </c>
+      <c r="B22">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C22">
+        <v>2.0356399999999999</v>
+      </c>
+      <c r="D22">
+        <v>3.2076E-2</v>
+      </c>
+      <c r="E22">
+        <v>3.2076000000000001E-4</v>
+      </c>
+      <c r="F22">
+        <v>0.39204</v>
+      </c>
+      <c r="G22">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.24</v>
+      </c>
+      <c r="B23">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C23">
+        <v>1.25156</v>
+      </c>
+      <c r="D23">
+        <v>3.2076E-2</v>
+      </c>
+      <c r="E23">
+        <v>3.2076000000000001E-4</v>
+      </c>
+      <c r="F23">
+        <v>0.39204</v>
+      </c>
+      <c r="G23">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B24">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C24">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D24">
+        <v>3.2076E-2</v>
+      </c>
+      <c r="E24">
+        <v>3.2076000000000001E-4</v>
+      </c>
+      <c r="F24">
+        <v>0.35283599999999998</v>
+      </c>
+      <c r="G24">
+        <v>432.24599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B25">
+        <v>2.6807599999999999E-3</v>
+      </c>
+      <c r="C25">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D25">
+        <v>3.5283599999999998E-2</v>
+      </c>
+      <c r="E25">
+        <v>3.2076000000000001E-4</v>
+      </c>
+      <c r="F25">
+        <v>0.35283599999999998</v>
+      </c>
+      <c r="G25">
+        <v>418.20600000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2.0392399999999999E-3</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1.6435999999999999</v>
+      </c>
+      <c r="D26" s="7">
+        <v>3.5283599999999998E-2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3.2076000000000001E-4</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.35283599999999998</v>
+      </c>
+      <c r="G26" s="7">
+        <v>418.20600000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.99644</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3.5283599999999998E-2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2.8868399999999999E-4</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.35283599999999998</v>
+      </c>
+      <c r="G27" s="5">
+        <v>418.20600000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.30736000000000002</v>
+      </c>
+      <c r="B28">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C28">
+        <v>1.99644</v>
+      </c>
+      <c r="D28">
+        <v>3.5283599999999998E-2</v>
+      </c>
+      <c r="E28">
+        <v>2.8868399999999999E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G28">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.236792</v>
+      </c>
+      <c r="B29">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C29">
+        <v>1.99644</v>
+      </c>
+      <c r="D29">
+        <v>3.5283599999999998E-2</v>
+      </c>
+      <c r="E29">
+        <v>2.8868399999999999E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G29">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B30">
+        <v>2.64868E-3</v>
+      </c>
+      <c r="C30">
+        <v>1.99644</v>
+      </c>
+      <c r="D30">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E30">
+        <v>2.8868399999999999E-4</v>
+      </c>
+      <c r="F30">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G30">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B31">
+        <v>2.0713200000000002E-3</v>
+      </c>
+      <c r="C31">
+        <v>1.99644</v>
+      </c>
+      <c r="D31">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E31">
+        <v>2.8868399999999999E-4</v>
+      </c>
+      <c r="F31">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G31">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B32">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C32">
+        <v>2.38456</v>
+      </c>
+      <c r="D32">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E32">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F32">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G32">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B33">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C33">
+        <v>1.60832</v>
+      </c>
+      <c r="D33">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E33">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F33">
+        <v>0.38812000000000002</v>
+      </c>
+      <c r="G33">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.30383100000000002</v>
+      </c>
+      <c r="B34">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C34">
+        <v>1.99644</v>
+      </c>
+      <c r="D34">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E34">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F34">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G34">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.24032100000000001</v>
+      </c>
+      <c r="B35">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C35">
+        <v>1.99644</v>
+      </c>
+      <c r="D35">
+        <v>3.1755199999999997E-2</v>
+      </c>
+      <c r="E35">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F35">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G35">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B36">
+        <v>2.6198200000000001E-3</v>
+      </c>
+      <c r="C36">
+        <v>1.99644</v>
+      </c>
+      <c r="D36">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E36">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F36">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G36">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B37">
+        <v>2.1001800000000001E-3</v>
+      </c>
+      <c r="C37">
+        <v>1.99644</v>
+      </c>
+      <c r="D37">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E37">
+        <v>2.5981600000000001E-4</v>
+      </c>
+      <c r="F37">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G37">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B38">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C38">
+        <v>2.3457400000000002</v>
+      </c>
+      <c r="D38">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E38">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F38">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G38">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B39">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C39">
+        <v>1.64713</v>
+      </c>
+      <c r="D39">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E39">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F39">
+        <v>0.34930800000000001</v>
+      </c>
+      <c r="G39">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.30065599999999998</v>
+      </c>
+      <c r="B40">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C40">
+        <v>1.99644</v>
+      </c>
+      <c r="D40">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E40">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F40">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G40">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.24349599999999999</v>
+      </c>
+      <c r="B41">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C41">
+        <v>1.99644</v>
+      </c>
+      <c r="D41">
+        <v>2.85797E-2</v>
+      </c>
+      <c r="E41">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F41">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G41">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B42">
+        <v>2.5938300000000001E-3</v>
+      </c>
+      <c r="C42">
+        <v>1.99644</v>
+      </c>
+      <c r="D42">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E42">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F42">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G42">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B43">
+        <v>2.1261700000000001E-3</v>
+      </c>
+      <c r="C43">
+        <v>1.99644</v>
+      </c>
+      <c r="D43">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E43">
+        <v>2.3383400000000001E-4</v>
+      </c>
+      <c r="F43">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G43">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B44">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C44">
+        <v>2.31081</v>
+      </c>
+      <c r="D44">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E44">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F44">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G44">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B45">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C45">
+        <v>1.6820600000000001</v>
+      </c>
+      <c r="D45">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E45">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F45">
+        <v>0.31437700000000002</v>
+      </c>
+      <c r="G45">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.29779800000000001</v>
+      </c>
+      <c r="B46">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C46">
+        <v>1.99644</v>
+      </c>
+      <c r="D46">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E46">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F46">
+        <v>0.282939</v>
+      </c>
+      <c r="G46">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.24635399999999999</v>
+      </c>
+      <c r="B47">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C47">
+        <v>1.99644</v>
+      </c>
+      <c r="D47">
+        <v>2.57217E-2</v>
+      </c>
+      <c r="E47">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F47">
+        <v>0.282939</v>
+      </c>
+      <c r="G47">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B48">
+        <v>2.5704500000000002E-3</v>
+      </c>
+      <c r="C48">
+        <v>1.99644</v>
+      </c>
+      <c r="D48">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E48">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F48">
+        <v>0.282939</v>
+      </c>
+      <c r="G48">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B49">
+        <v>2.1495500000000001E-3</v>
+      </c>
+      <c r="C49">
+        <v>1.99644</v>
+      </c>
+      <c r="D49">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E49">
+        <v>2.1045100000000001E-4</v>
+      </c>
+      <c r="F49">
+        <v>0.282939</v>
+      </c>
+      <c r="G49">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B50">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C50">
+        <v>2.2793800000000002</v>
+      </c>
+      <c r="D50">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E50">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F50">
+        <v>0.282939</v>
+      </c>
+      <c r="G50">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B51">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C51">
+        <v>1.7135</v>
+      </c>
+      <c r="D51">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E51">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F51">
+        <v>0.282939</v>
+      </c>
+      <c r="G51">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.29522599999999999</v>
+      </c>
+      <c r="B52">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C52">
+        <v>1.99644</v>
+      </c>
+      <c r="D52">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E52">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F52">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G52">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.24892600000000001</v>
+      </c>
+      <c r="B53">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C53">
+        <v>1.99644</v>
+      </c>
+      <c r="D53">
+        <v>2.3149599999999999E-2</v>
+      </c>
+      <c r="E53">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F53">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G53">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B54">
+        <v>2.5494099999999998E-3</v>
+      </c>
+      <c r="C54">
+        <v>1.99644</v>
+      </c>
+      <c r="D54">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E54">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F54">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G54">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B55">
+        <v>2.17059E-3</v>
+      </c>
+      <c r="C55">
+        <v>1.99644</v>
+      </c>
+      <c r="D55">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E55">
+        <v>1.8940600000000001E-4</v>
+      </c>
+      <c r="F55">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G55">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B56">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C56">
+        <v>2.25108</v>
+      </c>
+      <c r="D56">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E56">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F56">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G56">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B57">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C57">
+        <v>1.7417899999999999</v>
+      </c>
+      <c r="D57">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E57">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F57">
+        <v>0.25464500000000001</v>
+      </c>
+      <c r="G57">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.29291099999999998</v>
+      </c>
+      <c r="B58">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C58">
+        <v>1.99644</v>
+      </c>
+      <c r="D58">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E58">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F58">
+        <v>0.229181</v>
+      </c>
+      <c r="G58">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.25124099999999999</v>
+      </c>
+      <c r="B59">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C59">
+        <v>1.99644</v>
+      </c>
+      <c r="D59">
+        <v>2.0834600000000002E-2</v>
+      </c>
+      <c r="E59">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F59">
+        <v>0.229181</v>
+      </c>
+      <c r="G59">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B60">
+        <v>2.5304699999999999E-3</v>
+      </c>
+      <c r="C60">
+        <v>1.99644</v>
+      </c>
+      <c r="D60">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E60">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F60">
+        <v>0.229181</v>
+      </c>
+      <c r="G60">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B61">
+        <v>2.1895299999999999E-3</v>
+      </c>
+      <c r="C61">
+        <v>1.99644</v>
+      </c>
+      <c r="D61">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E61">
+        <v>1.7046499999999999E-4</v>
+      </c>
+      <c r="F61">
+        <v>0.229181</v>
+      </c>
+      <c r="G61">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B62">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C62">
+        <v>2.2256200000000002</v>
+      </c>
+      <c r="D62">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E62">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F62">
+        <v>0.229181</v>
+      </c>
+      <c r="G62">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B63">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C63">
+        <v>1.7672600000000001</v>
+      </c>
+      <c r="D63">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E63">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F63">
+        <v>0.229181</v>
+      </c>
+      <c r="G63">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0.290827</v>
+      </c>
+      <c r="B64">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C64">
+        <v>1.99644</v>
+      </c>
+      <c r="D64">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E64">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F64">
+        <v>0.206263</v>
+      </c>
+      <c r="G64">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.25332500000000002</v>
+      </c>
+      <c r="B65">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C65">
+        <v>1.99644</v>
+      </c>
+      <c r="D65">
+        <v>1.8751199999999999E-2</v>
+      </c>
+      <c r="E65">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F65">
+        <v>0.206263</v>
+      </c>
+      <c r="G65">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B66">
+        <v>2.5134200000000002E-3</v>
+      </c>
+      <c r="C66">
+        <v>1.99644</v>
+      </c>
+      <c r="D66">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E66">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F66">
+        <v>0.206263</v>
+      </c>
+      <c r="G66">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B67">
+        <v>2.2065800000000001E-3</v>
+      </c>
+      <c r="C67">
+        <v>1.99644</v>
+      </c>
+      <c r="D67">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E67">
+        <v>1.5341899999999999E-4</v>
+      </c>
+      <c r="F67">
+        <v>0.206263</v>
+      </c>
+      <c r="G67">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B68">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C68">
+        <v>2.2027000000000001</v>
+      </c>
+      <c r="D68">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E68">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F68">
+        <v>0.206263</v>
+      </c>
+      <c r="G68">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B69">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C69">
+        <v>1.79017</v>
+      </c>
+      <c r="D69">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E69">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F69">
+        <v>0.206263</v>
+      </c>
+      <c r="G69">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.28895199999999999</v>
+      </c>
+      <c r="B70">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C70">
+        <v>1.99644</v>
+      </c>
+      <c r="D70">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E70">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F70">
+        <v>0.185636</v>
+      </c>
+      <c r="G70">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0.25519999999999998</v>
+      </c>
+      <c r="B71">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C71">
+        <v>1.99644</v>
+      </c>
+      <c r="D71">
+        <v>1.6875999999999999E-2</v>
+      </c>
+      <c r="E71">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F71">
+        <v>0.185636</v>
+      </c>
+      <c r="G71">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B72">
+        <v>2.4980800000000002E-3</v>
+      </c>
+      <c r="C72">
+        <v>1.99644</v>
+      </c>
+      <c r="D72">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E72">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F72">
+        <v>0.185636</v>
+      </c>
+      <c r="G72">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B73">
+        <v>2.2219200000000001E-3</v>
+      </c>
+      <c r="C73">
+        <v>1.99644</v>
+      </c>
+      <c r="D73">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E73">
+        <v>1.3807700000000001E-4</v>
+      </c>
+      <c r="F73">
+        <v>0.185636</v>
+      </c>
+      <c r="G73">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B74">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C74">
+        <v>2.18207</v>
+      </c>
+      <c r="D74">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E74">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F74">
+        <v>0.185636</v>
+      </c>
+      <c r="G74">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B75">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C75">
+        <v>1.8108</v>
+      </c>
+      <c r="D75">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E75">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F75">
+        <v>0.185636</v>
+      </c>
+      <c r="G75">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.28726400000000002</v>
+      </c>
+      <c r="B76">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C76">
+        <v>1.99644</v>
+      </c>
+      <c r="D76">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E76">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F76">
+        <v>0.167073</v>
+      </c>
+      <c r="G76">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.25688800000000001</v>
+      </c>
+      <c r="B77">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C77">
+        <v>1.99644</v>
+      </c>
+      <c r="D77">
+        <v>1.5188399999999999E-2</v>
+      </c>
+      <c r="E77">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F77">
+        <v>0.167073</v>
+      </c>
+      <c r="G77">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B78">
+        <v>2.4842699999999998E-3</v>
+      </c>
+      <c r="C78">
+        <v>1.99644</v>
+      </c>
+      <c r="D78">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E78">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F78">
+        <v>0.167073</v>
+      </c>
+      <c r="G78">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B79">
+        <v>2.23573E-3</v>
+      </c>
+      <c r="C79">
+        <v>1.99644</v>
+      </c>
+      <c r="D79">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E79">
+        <v>1.2426900000000001E-4</v>
+      </c>
+      <c r="F79">
+        <v>0.167073</v>
+      </c>
+      <c r="G79">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B80">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C80">
+        <v>2.16351</v>
+      </c>
+      <c r="D80">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E80">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F80">
+        <v>0.167073</v>
+      </c>
+      <c r="G80">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B81">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C81">
+        <v>1.8293600000000001</v>
+      </c>
+      <c r="D81">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E81">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F81">
+        <v>0.167073</v>
+      </c>
+      <c r="G81">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.285746</v>
+      </c>
+      <c r="B82">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C82">
+        <v>1.99644</v>
+      </c>
+      <c r="D82">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E82">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F82">
+        <v>0.150365</v>
+      </c>
+      <c r="G82">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0.25840600000000002</v>
+      </c>
+      <c r="B83">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C83">
+        <v>1.99644</v>
+      </c>
+      <c r="D83">
+        <v>1.3669600000000001E-2</v>
+      </c>
+      <c r="E83">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F83">
+        <v>0.150365</v>
+      </c>
+      <c r="G83">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B84">
+        <v>2.4718399999999999E-3</v>
+      </c>
+      <c r="C84">
+        <v>1.99644</v>
+      </c>
+      <c r="D84">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E84">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F84">
+        <v>0.150365</v>
+      </c>
+      <c r="G84">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B85">
+        <v>2.2481599999999999E-3</v>
+      </c>
+      <c r="C85">
+        <v>1.99644</v>
+      </c>
+      <c r="D85">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E85">
+        <v>1.11842E-4</v>
+      </c>
+      <c r="F85">
+        <v>0.150365</v>
+      </c>
+      <c r="G85">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B86">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C86">
+        <v>2.1467999999999998</v>
+      </c>
+      <c r="D86">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E86">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F86">
+        <v>0.150365</v>
+      </c>
+      <c r="G86">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B87">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C87">
+        <v>1.8460700000000001</v>
+      </c>
+      <c r="D87">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E87">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F87">
+        <v>0.150365</v>
+      </c>
+      <c r="G87">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.28437899999999999</v>
+      </c>
+      <c r="B88">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C88">
+        <v>1.99644</v>
+      </c>
+      <c r="D88">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E88">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F88">
+        <v>0.135329</v>
+      </c>
+      <c r="G88">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0.25977299999999998</v>
+      </c>
+      <c r="B89">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C89">
+        <v>1.99644</v>
+      </c>
+      <c r="D89">
+        <v>1.23026E-2</v>
+      </c>
+      <c r="E89">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F89">
+        <v>0.135329</v>
+      </c>
+      <c r="G89">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B90">
+        <v>2.4606599999999999E-3</v>
+      </c>
+      <c r="C90">
+        <v>1.99644</v>
+      </c>
+      <c r="D90">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E90">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F90">
+        <v>0.135329</v>
+      </c>
+      <c r="G90">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B91">
+        <v>2.2593399999999999E-3</v>
+      </c>
+      <c r="C91">
+        <v>1.99644</v>
+      </c>
+      <c r="D91">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E91">
+        <v>1.00658E-4</v>
+      </c>
+      <c r="F91">
+        <v>0.135329</v>
+      </c>
+      <c r="G91">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B92">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C92">
+        <v>2.1317599999999999</v>
+      </c>
+      <c r="D92">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E92" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F92">
+        <v>0.135329</v>
+      </c>
+      <c r="G92">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B93">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C93">
+        <v>1.86111</v>
+      </c>
+      <c r="D93">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F93">
+        <v>0.135329</v>
+      </c>
+      <c r="G93">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0.28314800000000001</v>
+      </c>
+      <c r="B94">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C94">
+        <v>1.99644</v>
+      </c>
+      <c r="D94">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E94" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F94">
+        <v>0.121796</v>
+      </c>
+      <c r="G94">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0.26100400000000001</v>
+      </c>
+      <c r="B95">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C95">
+        <v>1.99644</v>
+      </c>
+      <c r="D95">
+        <v>1.10724E-2</v>
+      </c>
+      <c r="E95" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F95">
+        <v>0.121796</v>
+      </c>
+      <c r="G95">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B96">
+        <v>2.4505899999999999E-3</v>
+      </c>
+      <c r="C96">
+        <v>1.99644</v>
+      </c>
+      <c r="D96">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E96" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F96">
+        <v>0.121796</v>
+      </c>
+      <c r="G96">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B97">
+        <v>2.2694099999999999E-3</v>
+      </c>
+      <c r="C97">
+        <v>1.99644</v>
+      </c>
+      <c r="D97">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E97" s="1">
+        <v>9.0592099999999996E-5</v>
+      </c>
+      <c r="F97">
+        <v>0.121796</v>
+      </c>
+      <c r="G97">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B98">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C98">
+        <v>2.1182300000000001</v>
+      </c>
+      <c r="D98">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E98" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F98">
+        <v>0.121796</v>
+      </c>
+      <c r="G98">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B99">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C99">
+        <v>1.8746400000000001</v>
+      </c>
+      <c r="D99">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E99" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F99">
+        <v>0.121796</v>
+      </c>
+      <c r="G99">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0.28204099999999999</v>
+      </c>
+      <c r="B100">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C100">
+        <v>1.99644</v>
+      </c>
+      <c r="D100">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E100" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F100">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G100">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0.26211099999999998</v>
+      </c>
+      <c r="B101">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C101">
+        <v>1.99644</v>
+      </c>
+      <c r="D101">
+        <v>9.9651300000000009E-3</v>
+      </c>
+      <c r="E101" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F101">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G101">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B102">
+        <v>2.4415299999999999E-3</v>
+      </c>
+      <c r="C102">
+        <v>1.99644</v>
+      </c>
+      <c r="D102">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E102" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F102">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G102">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B103">
+        <v>2.2784699999999999E-3</v>
+      </c>
+      <c r="C103">
+        <v>1.99644</v>
+      </c>
+      <c r="D103">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E103" s="1">
+        <v>8.15329E-5</v>
+      </c>
+      <c r="F103">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G103">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B104">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C104">
+        <v>2.1060500000000002</v>
+      </c>
+      <c r="D104">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E104" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F104">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G104">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B105">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C105">
+        <v>1.8868199999999999</v>
+      </c>
+      <c r="D105">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E105" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F105">
+        <v>0.10961600000000001</v>
+      </c>
+      <c r="G105">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>0.28104499999999999</v>
+      </c>
+      <c r="B106">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C106">
+        <v>1.99644</v>
+      </c>
+      <c r="D106">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E106" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F106">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G106">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0.26310699999999998</v>
+      </c>
+      <c r="B107">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C107">
+        <v>1.99644</v>
+      </c>
+      <c r="D107">
+        <v>8.9686200000000001E-3</v>
+      </c>
+      <c r="E107" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F107">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G107">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B108">
+        <v>2.4333800000000002E-3</v>
+      </c>
+      <c r="C108">
+        <v>1.99644</v>
+      </c>
+      <c r="D108">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E108" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F108">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G108">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B109">
+        <v>2.2866200000000001E-3</v>
+      </c>
+      <c r="C109">
+        <v>1.99644</v>
+      </c>
+      <c r="D109">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E109" s="1">
+        <v>7.3379600000000005E-5</v>
+      </c>
+      <c r="F109">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G109">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B110">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C110">
+        <v>2.0950899999999999</v>
+      </c>
+      <c r="D110">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E110" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F110">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G110">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B111">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C111">
+        <v>1.89778</v>
+      </c>
+      <c r="D111">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E111" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F111">
+        <v>9.8654800000000001E-2</v>
+      </c>
+      <c r="G111">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>0.28014800000000001</v>
+      </c>
+      <c r="B112">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C112">
+        <v>1.99644</v>
+      </c>
+      <c r="D112">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E112" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F112">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G112">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>0.26400400000000002</v>
+      </c>
+      <c r="B113">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C113">
+        <v>1.99644</v>
+      </c>
+      <c r="D113">
+        <v>8.0717600000000007E-3</v>
+      </c>
+      <c r="E113" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F113">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G113">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B114">
+        <v>2.42604E-3</v>
+      </c>
+      <c r="C114">
+        <v>1.99644</v>
+      </c>
+      <c r="D114">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E114" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F114">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G114">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B115">
+        <v>2.2939599999999998E-3</v>
+      </c>
+      <c r="C115">
+        <v>1.99644</v>
+      </c>
+      <c r="D115">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E115" s="1">
+        <v>6.6041600000000001E-5</v>
+      </c>
+      <c r="F115">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G115">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B116">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C116">
+        <v>2.0852300000000001</v>
+      </c>
+      <c r="D116">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E116" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F116">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G116">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B117">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C117">
+        <v>1.9076500000000001</v>
+      </c>
+      <c r="D117">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E117" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F117">
+        <v>8.8789300000000002E-2</v>
+      </c>
+      <c r="G117">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>0.27934100000000001</v>
+      </c>
+      <c r="B118">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C118">
+        <v>1.99644</v>
+      </c>
+      <c r="D118">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E118" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F118">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G118">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>0.26481100000000002</v>
+      </c>
+      <c r="B119">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C119">
+        <v>1.99644</v>
+      </c>
+      <c r="D119">
+        <v>7.2645799999999996E-3</v>
+      </c>
+      <c r="E119" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F119">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G119">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B120">
+        <v>2.4194400000000001E-3</v>
+      </c>
+      <c r="C120">
+        <v>1.99644</v>
+      </c>
+      <c r="D120">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E120" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F120">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G120">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B121">
+        <v>2.3005600000000001E-3</v>
+      </c>
+      <c r="C121">
+        <v>1.99644</v>
+      </c>
+      <c r="D121">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E121" s="1">
+        <v>5.9437500000000001E-5</v>
+      </c>
+      <c r="F121">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G121">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B122">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C122">
+        <v>2.0763500000000001</v>
+      </c>
+      <c r="D122">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E122" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F122">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G122">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B123">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C123">
+        <v>1.9165300000000001</v>
+      </c>
+      <c r="D123">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E123" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F123">
+        <v>7.9910400000000006E-2</v>
+      </c>
+      <c r="G123">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>0.27861399999999997</v>
+      </c>
+      <c r="B124">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C124">
+        <v>1.99644</v>
+      </c>
+      <c r="D124">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E124" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F124">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G124">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>0.265538</v>
+      </c>
+      <c r="B125">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C125">
+        <v>1.99644</v>
+      </c>
+      <c r="D125">
+        <v>6.5381199999999997E-3</v>
+      </c>
+      <c r="E125" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F125">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G125">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B126">
+        <v>2.4134899999999999E-3</v>
+      </c>
+      <c r="C126">
+        <v>1.99644</v>
+      </c>
+      <c r="D126">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E126" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F126">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G126">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B127">
+        <v>2.3065099999999999E-3</v>
+      </c>
+      <c r="C127">
+        <v>1.99644</v>
+      </c>
+      <c r="D127">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E127" s="1">
+        <v>5.3493699999999999E-5</v>
+      </c>
+      <c r="F127">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G127">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B128">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C128">
+        <v>2.0683600000000002</v>
+      </c>
+      <c r="D128">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E128" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F128">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G128">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B129">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C129">
+        <v>1.92452</v>
+      </c>
+      <c r="D129">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E129" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F129">
+        <v>7.1919300000000005E-2</v>
+      </c>
+      <c r="G129">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>0.27795999999999998</v>
+      </c>
+      <c r="B130">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C130">
+        <v>1.99644</v>
+      </c>
+      <c r="D130">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E130" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F130">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G130">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>0.26619199999999998</v>
+      </c>
+      <c r="B131">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C131">
+        <v>1.99644</v>
+      </c>
+      <c r="D131">
+        <v>5.8843100000000002E-3</v>
+      </c>
+      <c r="E131" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F131">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G131">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B132">
+        <v>2.40814E-3</v>
+      </c>
+      <c r="C132">
+        <v>1.99644</v>
+      </c>
+      <c r="D132">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E132" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F132">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G132">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B133">
+        <v>2.3118599999999998E-3</v>
+      </c>
+      <c r="C133">
+        <v>1.99644</v>
+      </c>
+      <c r="D133">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E133" s="1">
+        <v>4.8144399999999999E-5</v>
+      </c>
+      <c r="F133">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G133">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B134">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C134">
+        <v>2.0611600000000001</v>
+      </c>
+      <c r="D134">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E134" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F134">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G134">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B135">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C135">
+        <v>1.93171</v>
+      </c>
+      <c r="D135">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E135" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F135">
+        <v>6.4727400000000004E-2</v>
+      </c>
+      <c r="G135">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>0.27737200000000001</v>
+      </c>
+      <c r="B136">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C136">
+        <v>1.99644</v>
+      </c>
+      <c r="D136">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E136" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F136">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G136">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>0.26678000000000002</v>
+      </c>
+      <c r="B137">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C137">
+        <v>1.99644</v>
+      </c>
+      <c r="D137">
+        <v>5.2958800000000002E-3</v>
+      </c>
+      <c r="E137" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F137">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G137">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B138">
+        <v>2.40333E-3</v>
+      </c>
+      <c r="C138">
+        <v>1.99644</v>
+      </c>
+      <c r="D138">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E138" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F138">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G138">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B139">
+        <v>2.3166699999999998E-3</v>
+      </c>
+      <c r="C139">
+        <v>1.99644</v>
+      </c>
+      <c r="D139">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E139" s="1">
+        <v>4.33299E-5</v>
+      </c>
+      <c r="F139">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G139">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B140">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C140">
+        <v>2.0546899999999999</v>
+      </c>
+      <c r="D140">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E140" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F140">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G140">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B141">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C141">
+        <v>1.93818</v>
+      </c>
+      <c r="D141">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E141" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F141">
+        <v>5.82547E-2</v>
+      </c>
+      <c r="G141">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0.27684199999999998</v>
+      </c>
+      <c r="B142">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C142">
+        <v>1.99644</v>
+      </c>
+      <c r="D142">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E142" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F142">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G142">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>0.26730999999999999</v>
+      </c>
+      <c r="B143">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C143">
+        <v>1.99644</v>
+      </c>
+      <c r="D143">
+        <v>4.7662900000000003E-3</v>
+      </c>
+      <c r="E143" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F143">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G143">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B144">
+        <v>2.3990000000000001E-3</v>
+      </c>
+      <c r="C144">
+        <v>1.99644</v>
+      </c>
+      <c r="D144">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E144" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F144">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G144">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B145">
+        <v>2.3210000000000001E-3</v>
+      </c>
+      <c r="C145">
+        <v>1.99644</v>
+      </c>
+      <c r="D145">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E145" s="1">
+        <v>3.8996899999999999E-5</v>
+      </c>
+      <c r="F145">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G145">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B146">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C146">
+        <v>2.04887</v>
+      </c>
+      <c r="D146">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E146" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F146">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G146">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B147">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C147">
+        <v>1.94401</v>
+      </c>
+      <c r="D147">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E147" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F147">
+        <v>5.2429200000000002E-2</v>
+      </c>
+      <c r="G147">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>0.276366</v>
+      </c>
+      <c r="B148">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C148">
+        <v>1.99644</v>
+      </c>
+      <c r="D148">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E148" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F148">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G148">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>0.26778600000000002</v>
+      </c>
+      <c r="B149">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C149">
+        <v>1.99644</v>
+      </c>
+      <c r="D149">
+        <v>4.2896599999999998E-3</v>
+      </c>
+      <c r="E149" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F149">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G149">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B150">
+        <v>2.3950999999999998E-3</v>
+      </c>
+      <c r="C150">
+        <v>1.99644</v>
+      </c>
+      <c r="D150">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E150" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F150">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G150">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B151">
+        <v>2.3249E-3</v>
+      </c>
+      <c r="C151">
+        <v>1.99644</v>
+      </c>
+      <c r="D151">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E151" s="1">
+        <v>3.50972E-5</v>
+      </c>
+      <c r="F151">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G151">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B152">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C152">
+        <v>2.0436200000000002</v>
+      </c>
+      <c r="D152">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E152" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F152">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G152">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B153">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C153">
+        <v>1.9492499999999999</v>
+      </c>
+      <c r="D153">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E153" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F153">
+        <v>4.71863E-2</v>
+      </c>
+      <c r="G153">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>0.27593699999999999</v>
+      </c>
+      <c r="B154">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C154">
+        <v>1.99644</v>
+      </c>
+      <c r="D154">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E154" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F154">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G154">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>0.26821499999999998</v>
+      </c>
+      <c r="B155">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C155">
+        <v>1.99644</v>
+      </c>
+      <c r="D155">
+        <v>3.8606999999999999E-3</v>
+      </c>
+      <c r="E155" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F155">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G155">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B156">
+        <v>2.3915899999999999E-3</v>
+      </c>
+      <c r="C156">
+        <v>1.99644</v>
+      </c>
+      <c r="D156">
+        <v>3.4746299999999998E-3</v>
+      </c>
+      <c r="E156" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F156">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G156">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B157">
+        <v>2.3284099999999999E-3</v>
+      </c>
+      <c r="C157">
+        <v>1.99644</v>
+      </c>
+      <c r="D157">
+        <v>3.4746299999999998E-3</v>
+      </c>
+      <c r="E157" s="1">
+        <v>3.1587500000000002E-5</v>
+      </c>
+      <c r="F157">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G157">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B158">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C158">
+        <v>2.0388999999999999</v>
+      </c>
+      <c r="D158">
+        <v>3.4746299999999998E-3</v>
+      </c>
+      <c r="E158" s="1">
+        <v>2.8428800000000001E-5</v>
+      </c>
+      <c r="F158">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G158">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>0.27207599999999998</v>
+      </c>
+      <c r="B159">
+        <v>2.3600000000000001E-3</v>
+      </c>
+      <c r="C159">
+        <v>1.95397</v>
+      </c>
+      <c r="D159">
+        <v>3.4746299999999998E-3</v>
+      </c>
+      <c r="E159" s="1">
+        <v>2.8428800000000001E-5</v>
+      </c>
+      <c r="F159">
+        <v>4.2467699999999997E-2</v>
+      </c>
+      <c r="G159">
+        <v>402.42899999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>